<commit_message>
TP-6 added assets in confing file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIpath_projects\TripPlanner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE93CCF-2453-4755-B47F-8AE0223EA329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -160,13 +160,37 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>EmailCredentials</t>
+  </si>
+  <si>
+    <t>GoogleFormLink</t>
+  </si>
+  <si>
+    <t>LetterSubject</t>
+  </si>
+  <si>
+    <t>LetterText</t>
+  </si>
+  <si>
+    <t>This is credentials for email in which we receive registration letters from users, and from which we send responses and new data about trips.</t>
+  </si>
+  <si>
+    <t>This is link to google form that any user of trip-planner need to fulfill to provide</t>
+  </si>
+  <si>
+    <t>Text that will be send for each user who would like to start registration in trip-planner</t>
+  </si>
+  <si>
+    <t>Trip-Planner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +214,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,6 +252,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2782,7 +2814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2828,10 +2862,59 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3830,5 +3913,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TP-14 added response send robot
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIpath_projects\TripPlanner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE93CCF-2453-4755-B47F-8AE0223EA329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F33525-927A-4046-8D5A-CC22DB1986D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -183,7 +183,7 @@
     <t>Text that will be send for each user who would like to start registration in trip-planner</t>
   </si>
   <si>
-    <t>Trip-Planner</t>
+    <t xml:space="preserve">Trip-Planner Robot Registration Response Letter Subject </t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -647,10 +647,50 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2815,7 +2855,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2863,57 +2903,21 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Synchronise with the latest version of the develop branch
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIpath_projects\TripPlanner\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F33525-927A-4046-8D5A-CC22DB1986D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -160,37 +160,13 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>EmailCredentials</t>
-  </si>
-  <si>
-    <t>GoogleFormLink</t>
-  </si>
-  <si>
-    <t>LetterSubject</t>
-  </si>
-  <si>
-    <t>LetterText</t>
-  </si>
-  <si>
-    <t>This is credentials for email in which we receive registration letters from users, and from which we send responses and new data about trips.</t>
-  </si>
-  <si>
-    <t>This is link to google form that any user of trip-planner need to fulfill to provide</t>
-  </si>
-  <si>
-    <t>Text that will be send for each user who would like to start registration in trip-planner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trip-Planner Robot Registration Response Letter Subject </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,13 +190,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -242,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -252,7 +221,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -647,50 +615,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2854,9 +2782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2902,23 +2828,10 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3917,6 +3830,5 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>